<commit_message>
new Dashboard Testing sheet is added
</commit_message>
<xml_diff>
--- a/Trakeme_Dashboard_testing.xlsx
+++ b/Trakeme_Dashboard_testing.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\trakemeTesting_Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trakme_Testing_report\Manual_Testing_sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24D660B-BABA-4845-B9C5-530F89C7D7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A231BB90-8C11-4654-A6FC-F30FF3C84D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{48BE6045-7B4F-4F23-A95D-99C368872939}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dashboard1.1" sheetId="3" r:id="rId1"/>
-    <sheet name="Dashboard1.0" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="Dashboard1.2" sheetId="4" r:id="rId1"/>
+    <sheet name="Dashboard1.1" sheetId="3" r:id="rId2"/>
+    <sheet name="Dashboard1.0" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="92">
   <si>
     <t>Project Name</t>
   </si>
@@ -146,9 +145,6 @@
   </si>
   <si>
     <t>Ensure that the user's name and role (if dynamic) are displayed as expected.</t>
-  </si>
-  <si>
-    <t>bsnl logo should be there</t>
   </si>
   <si>
     <t>hamburger  should be available</t>
@@ -309,6 +305,15 @@
   </si>
   <si>
     <t xml:space="preserve">On clicking next button,page scrolls down. </t>
+  </si>
+  <si>
+    <t>Link Not availble</t>
+  </si>
+  <si>
+    <t>It should work properly</t>
+  </si>
+  <si>
+    <t>Inserting different details for searching</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1056,21 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1409,11 +1428,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{943C1E70-5421-440C-999F-9C5302E2B928}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A98B6E3C-6190-427D-98ED-77CAC4DE1233}">
   <dimension ref="C4:V41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H19" zoomScale="94" workbookViewId="0">
-      <selection activeCell="U34" sqref="U34"/>
+    <sheetView tabSelected="1" topLeftCell="M36" zoomScale="99" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23:U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1500,7 +1519,9 @@
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="3">
+        <v>45007</v>
+      </c>
     </row>
     <row r="12" spans="3:22" ht="29" x14ac:dyDescent="0.35">
       <c r="K12" s="4" t="s">
@@ -1557,7 +1578,7 @@
         <v>26</v>
       </c>
       <c r="P13" s="88" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q13" s="89" t="s">
         <v>28</v>
@@ -1569,7 +1590,7 @@
         <v>4</v>
       </c>
       <c r="T13" s="80">
-        <v>45309</v>
+        <v>45007</v>
       </c>
       <c r="U13" s="82"/>
       <c r="V13" s="41"/>
@@ -1619,7 +1640,7 @@
         <v>4</v>
       </c>
       <c r="T15" s="37">
-        <v>45309</v>
+        <v>45007</v>
       </c>
       <c r="U15" s="39"/>
       <c r="V15" s="41"/>
@@ -1633,9 +1654,7 @@
       </c>
       <c r="O16" s="77"/>
       <c r="P16" s="61"/>
-      <c r="Q16" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="Q16" s="9"/>
       <c r="R16" s="43"/>
       <c r="S16" s="43"/>
       <c r="T16" s="44"/>
@@ -1650,7 +1669,7 @@
       <c r="O17" s="74"/>
       <c r="P17" s="56"/>
       <c r="Q17" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R17" s="36"/>
       <c r="S17" s="36"/>
@@ -1663,13 +1682,13 @@
         <v>22</v>
       </c>
       <c r="L18" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="M18" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="M18" s="71" t="s">
+      <c r="N18" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="N18" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="O18" s="73" t="s">
         <v>27</v>
@@ -1678,7 +1697,7 @@
         <v>27</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R18" s="35" t="s">
         <v>29</v>
@@ -1687,7 +1706,7 @@
         <v>4</v>
       </c>
       <c r="T18" s="37">
-        <v>45309</v>
+        <v>45007</v>
       </c>
       <c r="U18" s="39"/>
       <c r="V18" s="41"/>
@@ -1697,12 +1716,12 @@
       <c r="L19" s="58"/>
       <c r="M19" s="76"/>
       <c r="N19" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O19" s="77"/>
       <c r="P19" s="61"/>
       <c r="Q19" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R19" s="43"/>
       <c r="S19" s="43"/>
@@ -1715,12 +1734,12 @@
       <c r="L20" s="50"/>
       <c r="M20" s="72"/>
       <c r="N20" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O20" s="74"/>
       <c r="P20" s="56"/>
       <c r="Q20" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R20" s="36"/>
       <c r="S20" s="36"/>
@@ -1733,20 +1752,20 @@
         <v>22</v>
       </c>
       <c r="L21" s="49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M21" s="71" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O21" s="73"/>
       <c r="P21" s="55" t="s">
         <v>27</v>
       </c>
       <c r="Q21" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R21" s="35" t="s">
         <v>29</v>
@@ -1755,10 +1774,10 @@
         <v>4</v>
       </c>
       <c r="T21" s="37">
-        <v>45309</v>
+        <v>45007</v>
       </c>
       <c r="U21" s="39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V21" s="41"/>
     </row>
@@ -1767,7 +1786,7 @@
       <c r="L22" s="50"/>
       <c r="M22" s="72"/>
       <c r="N22" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O22" s="74"/>
       <c r="P22" s="56"/>
@@ -1780,16 +1799,16 @@
     </row>
     <row r="23" spans="11:22" ht="121.5" x14ac:dyDescent="0.35">
       <c r="K23" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="L23" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="L23" s="49" t="s">
+      <c r="M23" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="M23" s="51" t="s">
-        <v>51</v>
-      </c>
       <c r="N23" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O23" s="66"/>
       <c r="P23" s="55" t="s">
@@ -1803,11 +1822,9 @@
         <v>4</v>
       </c>
       <c r="T23" s="37">
-        <v>45309</v>
-      </c>
-      <c r="U23" s="39" t="s">
-        <v>88</v>
-      </c>
+        <v>45007</v>
+      </c>
+      <c r="U23" s="39"/>
       <c r="V23" s="41"/>
     </row>
     <row r="24" spans="11:22" ht="54" x14ac:dyDescent="0.35">
@@ -1815,7 +1832,7 @@
       <c r="L24" s="58"/>
       <c r="M24" s="59"/>
       <c r="N24" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O24" s="67"/>
       <c r="P24" s="61"/>
@@ -1831,7 +1848,7 @@
       <c r="L25" s="58"/>
       <c r="M25" s="59"/>
       <c r="N25" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O25" s="67"/>
       <c r="P25" s="61"/>
@@ -1847,7 +1864,7 @@
       <c r="L26" s="50"/>
       <c r="M26" s="52"/>
       <c r="N26" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O26" s="68"/>
       <c r="P26" s="56"/>
@@ -1860,16 +1877,16 @@
     </row>
     <row r="27" spans="11:22" ht="54" x14ac:dyDescent="0.35">
       <c r="K27" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="L27" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="M27" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="L27" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="M27" s="51" t="s">
-        <v>56</v>
-      </c>
       <c r="N27" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O27" s="53"/>
       <c r="P27" s="55" t="s">
@@ -1883,11 +1900,9 @@
         <v>4</v>
       </c>
       <c r="T27" s="37">
-        <v>45309</v>
-      </c>
-      <c r="U27" s="39" t="s">
-        <v>87</v>
-      </c>
+        <v>45007</v>
+      </c>
+      <c r="U27" s="39"/>
       <c r="V27" s="41"/>
     </row>
     <row r="28" spans="11:22" ht="40.5" x14ac:dyDescent="0.35">
@@ -1895,7 +1910,7 @@
       <c r="L28" s="58"/>
       <c r="M28" s="59"/>
       <c r="N28" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O28" s="60"/>
       <c r="P28" s="61"/>
@@ -1911,7 +1926,7 @@
       <c r="L29" s="58"/>
       <c r="M29" s="59"/>
       <c r="N29" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O29" s="60"/>
       <c r="P29" s="61"/>
@@ -1952,16 +1967,16 @@
     </row>
     <row r="32" spans="11:22" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K32" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="L32" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="L32" s="49" t="s">
+      <c r="M32" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="M32" s="51" t="s">
+      <c r="N32" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="N32" s="8" t="s">
-        <v>60</v>
       </c>
       <c r="O32" s="53"/>
       <c r="P32" s="55" t="s">
@@ -1975,9 +1990,11 @@
         <v>4</v>
       </c>
       <c r="T32" s="37">
-        <v>45309</v>
-      </c>
-      <c r="U32" s="39"/>
+        <v>45007</v>
+      </c>
+      <c r="U32" s="39" t="s">
+        <v>89</v>
+      </c>
       <c r="V32" s="41"/>
     </row>
     <row r="33" spans="11:22" ht="89.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1985,7 +2002,7 @@
       <c r="L33" s="50"/>
       <c r="M33" s="52"/>
       <c r="N33" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O33" s="54"/>
       <c r="P33" s="56"/>
@@ -1998,52 +2015,54 @@
     </row>
     <row r="34" spans="11:22" ht="81.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K34" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="L34" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="M34" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="L34" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="M34" s="12" t="s">
-        <v>63</v>
-      </c>
       <c r="N34" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O34" s="15"/>
       <c r="P34" s="16"/>
       <c r="Q34" s="17"/>
       <c r="R34" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="S34" s="7" t="s">
         <v>4</v>
       </c>
       <c r="T34" s="28">
-        <v>45309</v>
+        <v>45007</v>
       </c>
       <c r="U34" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V34" s="18"/>
     </row>
-    <row r="35" spans="11:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="11:22" ht="27.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K35" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L35" s="14"/>
       <c r="M35" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N35" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O35" s="6"/>
       <c r="P35" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q35" s="7"/>
+        <v>91</v>
+      </c>
+      <c r="Q35" s="7" t="s">
+        <v>90</v>
+      </c>
       <c r="R35" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S35" s="7"/>
       <c r="T35" s="7"/>
@@ -2052,11 +2071,11 @@
     </row>
     <row r="36" spans="11:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K36" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L36" s="14"/>
       <c r="M36" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N36" s="10"/>
       <c r="O36" s="6"/>
@@ -2070,11 +2089,11 @@
     </row>
     <row r="37" spans="11:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K37" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L37" s="14"/>
       <c r="M37" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N37" s="19"/>
       <c r="O37" s="20"/>
@@ -2088,7 +2107,7 @@
     </row>
     <row r="41" spans="11:22" x14ac:dyDescent="0.35">
       <c r="K41" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L41" s="32"/>
       <c r="M41" s="32"/>
@@ -2183,6 +2202,793 @@
     <mergeCell ref="P32:P33"/>
   </mergeCells>
   <conditionalFormatting sqref="R13:T37">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",R13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",R13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="P13" r:id="rId1" xr:uid="{9DE33481-00DE-4FCB-9C9A-DE317731343B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{943C1E70-5421-440C-999F-9C5302E2B928}">
+  <dimension ref="C4:V41"/>
+  <sheetViews>
+    <sheetView topLeftCell="N28" zoomScale="53" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.26953125" customWidth="1"/>
+    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.26953125" customWidth="1"/>
+    <col min="16" max="16" width="22.1796875" customWidth="1"/>
+    <col min="17" max="17" width="23.90625" customWidth="1"/>
+    <col min="18" max="18" width="31.54296875" style="23" customWidth="1"/>
+    <col min="19" max="19" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:22" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" s="84" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="84"/>
+      <c r="R4" s="84"/>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.35">
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="84"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="84"/>
+      <c r="R5" s="84"/>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.35">
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" s="84"/>
+      <c r="P6" s="84"/>
+      <c r="Q6" s="84"/>
+      <c r="R6" s="84"/>
+    </row>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.35">
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45301</v>
+      </c>
+      <c r="O7" s="84"/>
+      <c r="P7" s="84"/>
+      <c r="Q7" s="84"/>
+      <c r="R7" s="84"/>
+    </row>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.35">
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O8" s="84"/>
+      <c r="P8" s="84"/>
+      <c r="Q8" s="84"/>
+      <c r="R8" s="84"/>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.35">
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="12" spans="3:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="K12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R12" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U12" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="3:22" x14ac:dyDescent="0.35">
+      <c r="K13" s="85" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="86" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" s="88" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q13" s="89" t="s">
+        <v>28</v>
+      </c>
+      <c r="R13" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="S13" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="T13" s="80">
+        <v>45309</v>
+      </c>
+      <c r="U13" s="82"/>
+      <c r="V13" s="41"/>
+    </row>
+    <row r="14" spans="3:22" ht="27.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K14" s="70"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="72"/>
+      <c r="N14" s="72"/>
+      <c r="O14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" s="56"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="79"/>
+      <c r="S14" s="79"/>
+      <c r="T14" s="81"/>
+      <c r="U14" s="83"/>
+      <c r="V14" s="42"/>
+    </row>
+    <row r="15" spans="3:22" ht="27" x14ac:dyDescent="0.35">
+      <c r="K15" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O15" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="P15" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="R15" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="S15" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="T15" s="37">
+        <v>45309</v>
+      </c>
+      <c r="U15" s="39"/>
+      <c r="V15" s="41"/>
+    </row>
+    <row r="16" spans="3:22" ht="67.5" x14ac:dyDescent="0.35">
+      <c r="K16" s="75"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="76"/>
+      <c r="N16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="O16" s="77"/>
+      <c r="P16" s="61"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="43"/>
+      <c r="S16" s="43"/>
+      <c r="T16" s="44"/>
+      <c r="U16" s="45"/>
+      <c r="V16" s="46"/>
+    </row>
+    <row r="17" spans="11:22" ht="27.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K17" s="70"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="72"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="74"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="38"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="42"/>
+    </row>
+    <row r="18" spans="11:22" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="K18" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="M18" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="P18" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="R18" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="S18" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="T18" s="37">
+        <v>45309</v>
+      </c>
+      <c r="U18" s="39"/>
+      <c r="V18" s="41"/>
+    </row>
+    <row r="19" spans="11:22" ht="54" x14ac:dyDescent="0.35">
+      <c r="K19" s="75"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="76"/>
+      <c r="N19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="O19" s="77"/>
+      <c r="P19" s="61"/>
+      <c r="Q19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="R19" s="43"/>
+      <c r="S19" s="43"/>
+      <c r="T19" s="44"/>
+      <c r="U19" s="45"/>
+      <c r="V19" s="46"/>
+    </row>
+    <row r="20" spans="11:22" ht="54.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K20" s="70"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="72"/>
+      <c r="N20" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="O20" s="74"/>
+      <c r="P20" s="56"/>
+      <c r="Q20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="R20" s="36"/>
+      <c r="S20" s="36"/>
+      <c r="T20" s="38"/>
+      <c r="U20" s="40"/>
+      <c r="V20" s="42"/>
+    </row>
+    <row r="21" spans="11:22" ht="67.5" x14ac:dyDescent="0.35">
+      <c r="K21" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="M21" s="71" t="s">
+        <v>45</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="O21" s="73"/>
+      <c r="P21" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q21" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="R21" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="S21" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="T21" s="37">
+        <v>45309</v>
+      </c>
+      <c r="U21" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="V21" s="41"/>
+    </row>
+    <row r="22" spans="11:22" ht="68" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K22" s="70"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="72"/>
+      <c r="N22" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O22" s="74"/>
+      <c r="P22" s="56"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="38"/>
+      <c r="U22" s="40"/>
+      <c r="V22" s="42"/>
+    </row>
+    <row r="23" spans="11:22" ht="121.5" x14ac:dyDescent="0.35">
+      <c r="K23" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="L23" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="M23" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="N23" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="O23" s="66"/>
+      <c r="P23" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q23" s="63"/>
+      <c r="R23" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="S23" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="T23" s="37">
+        <v>45309</v>
+      </c>
+      <c r="U23" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="V23" s="41"/>
+    </row>
+    <row r="24" spans="11:22" ht="54" x14ac:dyDescent="0.35">
+      <c r="K24" s="57"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="59"/>
+      <c r="N24" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="O24" s="67"/>
+      <c r="P24" s="61"/>
+      <c r="Q24" s="64"/>
+      <c r="R24" s="43"/>
+      <c r="S24" s="43"/>
+      <c r="T24" s="44"/>
+      <c r="U24" s="45"/>
+      <c r="V24" s="46"/>
+    </row>
+    <row r="25" spans="11:22" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="K25" s="57"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="O25" s="67"/>
+      <c r="P25" s="61"/>
+      <c r="Q25" s="64"/>
+      <c r="R25" s="43"/>
+      <c r="S25" s="43"/>
+      <c r="T25" s="44"/>
+      <c r="U25" s="45"/>
+      <c r="V25" s="46"/>
+    </row>
+    <row r="26" spans="11:22" ht="54.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K26" s="48"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="52"/>
+      <c r="N26" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="O26" s="68"/>
+      <c r="P26" s="56"/>
+      <c r="Q26" s="65"/>
+      <c r="R26" s="36"/>
+      <c r="S26" s="36"/>
+      <c r="T26" s="38"/>
+      <c r="U26" s="40"/>
+      <c r="V26" s="42"/>
+    </row>
+    <row r="27" spans="11:22" ht="54" x14ac:dyDescent="0.35">
+      <c r="K27" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="L27" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="M27" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="N27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O27" s="53"/>
+      <c r="P27" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q27" s="33"/>
+      <c r="R27" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="S27" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="T27" s="37">
+        <v>45309</v>
+      </c>
+      <c r="U27" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="V27" s="41"/>
+    </row>
+    <row r="28" spans="11:22" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="K28" s="57"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="59"/>
+      <c r="N28" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="O28" s="60"/>
+      <c r="P28" s="61"/>
+      <c r="Q28" s="62"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="43"/>
+      <c r="T28" s="44"/>
+      <c r="U28" s="45"/>
+      <c r="V28" s="46"/>
+    </row>
+    <row r="29" spans="11:22" ht="67.5" x14ac:dyDescent="0.35">
+      <c r="K29" s="57"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="O29" s="60"/>
+      <c r="P29" s="61"/>
+      <c r="Q29" s="62"/>
+      <c r="R29" s="43"/>
+      <c r="S29" s="43"/>
+      <c r="T29" s="44"/>
+      <c r="U29" s="45"/>
+      <c r="V29" s="46"/>
+    </row>
+    <row r="30" spans="11:22" x14ac:dyDescent="0.35">
+      <c r="K30" s="57"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="59"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="60"/>
+      <c r="P30" s="61"/>
+      <c r="Q30" s="62"/>
+      <c r="R30" s="43"/>
+      <c r="S30" s="43"/>
+      <c r="T30" s="44"/>
+      <c r="U30" s="45"/>
+      <c r="V30" s="46"/>
+    </row>
+    <row r="31" spans="11:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K31" s="48"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="52"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="54"/>
+      <c r="P31" s="56"/>
+      <c r="Q31" s="34"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="36"/>
+      <c r="T31" s="38"/>
+      <c r="U31" s="40"/>
+      <c r="V31" s="42"/>
+    </row>
+    <row r="32" spans="11:22" ht="84" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K32" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="L32" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="M32" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="N32" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="O32" s="53"/>
+      <c r="P32" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q32" s="33"/>
+      <c r="R32" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="S32" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="T32" s="37">
+        <v>45309</v>
+      </c>
+      <c r="U32" s="39"/>
+      <c r="V32" s="41"/>
+    </row>
+    <row r="33" spans="11:22" ht="89.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K33" s="48"/>
+      <c r="L33" s="50"/>
+      <c r="M33" s="52"/>
+      <c r="N33" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="O33" s="54"/>
+      <c r="P33" s="56"/>
+      <c r="Q33" s="34"/>
+      <c r="R33" s="36"/>
+      <c r="S33" s="36"/>
+      <c r="T33" s="38"/>
+      <c r="U33" s="40"/>
+      <c r="V33" s="42"/>
+    </row>
+    <row r="34" spans="11:22" ht="81.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K34" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="L34" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="M34" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="N34" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O34" s="15"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="S34" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="T34" s="28">
+        <v>45309</v>
+      </c>
+      <c r="U34" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="V34" s="18"/>
+    </row>
+    <row r="35" spans="11:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K35" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="L35" s="14"/>
+      <c r="M35" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="N35" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="O35" s="6"/>
+      <c r="P35" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="31"/>
+      <c r="V35" s="18"/>
+    </row>
+    <row r="36" spans="11:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K36" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="L36" s="14"/>
+      <c r="M36" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="N36" s="10"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="31"/>
+      <c r="V36" s="18"/>
+    </row>
+    <row r="37" spans="11:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K37" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="L37" s="14"/>
+      <c r="M37" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N37" s="19"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+      <c r="U37" s="31"/>
+      <c r="V37" s="18"/>
+    </row>
+    <row r="41" spans="11:22" x14ac:dyDescent="0.35">
+      <c r="K41" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="L41" s="32"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="32"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
+      <c r="S41" s="32"/>
+      <c r="T41" s="32"/>
+      <c r="U41" s="32"/>
+      <c r="V41" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="77">
+    <mergeCell ref="O4:R8"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="O15:O17"/>
+    <mergeCell ref="P15:P17"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="S15:S17"/>
+    <mergeCell ref="T15:T17"/>
+    <mergeCell ref="U15:U17"/>
+    <mergeCell ref="V15:V17"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="L18:L20"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="O18:O20"/>
+    <mergeCell ref="P18:P20"/>
+    <mergeCell ref="R18:R20"/>
+    <mergeCell ref="S18:S20"/>
+    <mergeCell ref="T18:T20"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="V18:V20"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="K23:K26"/>
+    <mergeCell ref="L23:L26"/>
+    <mergeCell ref="M23:M26"/>
+    <mergeCell ref="O23:O26"/>
+    <mergeCell ref="P23:P26"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="U23:U26"/>
+    <mergeCell ref="V23:V26"/>
+    <mergeCell ref="R21:R22"/>
+    <mergeCell ref="S21:S22"/>
+    <mergeCell ref="T21:T22"/>
+    <mergeCell ref="U21:U22"/>
+    <mergeCell ref="V21:V22"/>
+    <mergeCell ref="R23:R26"/>
+    <mergeCell ref="S23:S26"/>
+    <mergeCell ref="T23:T26"/>
+    <mergeCell ref="R27:R31"/>
+    <mergeCell ref="S27:S31"/>
+    <mergeCell ref="T27:T31"/>
+    <mergeCell ref="M27:M31"/>
+    <mergeCell ref="O27:O31"/>
+    <mergeCell ref="P27:P31"/>
+    <mergeCell ref="Q27:Q31"/>
+    <mergeCell ref="Q23:Q26"/>
+    <mergeCell ref="U27:U31"/>
+    <mergeCell ref="V27:V31"/>
+    <mergeCell ref="K41:V41"/>
+    <mergeCell ref="Q32:Q33"/>
+    <mergeCell ref="R32:R33"/>
+    <mergeCell ref="S32:S33"/>
+    <mergeCell ref="T32:T33"/>
+    <mergeCell ref="U32:U33"/>
+    <mergeCell ref="V32:V33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="O32:O33"/>
+    <mergeCell ref="P32:P33"/>
+    <mergeCell ref="K27:K31"/>
+    <mergeCell ref="L27:L31"/>
+  </mergeCells>
+  <conditionalFormatting sqref="R13:T37">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",R13)))</formula>
     </cfRule>
@@ -2197,12 +3003,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0075A1-D0CE-4894-BAFB-8A14606FB747}">
   <dimension ref="C4:V41"/>
   <sheetViews>
-    <sheetView topLeftCell="G50" zoomScale="63" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41:V41"/>
+    <sheetView topLeftCell="B1" zoomScale="63" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2346,7 +3152,7 @@
         <v>26</v>
       </c>
       <c r="P13" s="88" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q13" s="89" t="s">
         <v>28</v>
@@ -2422,9 +3228,7 @@
       </c>
       <c r="O16" s="77"/>
       <c r="P16" s="61"/>
-      <c r="Q16" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="Q16" s="9"/>
       <c r="R16" s="43"/>
       <c r="S16" s="43"/>
       <c r="T16" s="44"/>
@@ -2439,7 +3243,7 @@
       <c r="O17" s="74"/>
       <c r="P17" s="56"/>
       <c r="Q17" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R17" s="36"/>
       <c r="S17" s="36"/>
@@ -2452,13 +3256,13 @@
         <v>22</v>
       </c>
       <c r="L18" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="M18" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="M18" s="71" t="s">
+      <c r="N18" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="N18" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="O18" s="73" t="s">
         <v>27</v>
@@ -2467,7 +3271,7 @@
         <v>27</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R18" s="35" t="s">
         <v>29</v>
@@ -2486,12 +3290,12 @@
       <c r="L19" s="58"/>
       <c r="M19" s="76"/>
       <c r="N19" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O19" s="77"/>
       <c r="P19" s="61"/>
       <c r="Q19" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R19" s="43"/>
       <c r="S19" s="43"/>
@@ -2504,12 +3308,12 @@
       <c r="L20" s="50"/>
       <c r="M20" s="72"/>
       <c r="N20" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O20" s="74"/>
       <c r="P20" s="56"/>
       <c r="Q20" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R20" s="36"/>
       <c r="S20" s="36"/>
@@ -2522,23 +3326,23 @@
         <v>22</v>
       </c>
       <c r="L21" s="49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M21" s="71" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O21" s="73"/>
       <c r="P21" s="55" t="s">
         <v>27</v>
       </c>
       <c r="Q21" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R21" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S21" s="35" t="s">
         <v>4</v>
@@ -2554,7 +3358,7 @@
       <c r="L22" s="50"/>
       <c r="M22" s="72"/>
       <c r="N22" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O22" s="74"/>
       <c r="P22" s="56"/>
@@ -2567,16 +3371,16 @@
     </row>
     <row r="23" spans="11:22" ht="135" x14ac:dyDescent="0.35">
       <c r="K23" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="L23" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="L23" s="49" t="s">
+      <c r="M23" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="M23" s="51" t="s">
-        <v>51</v>
-      </c>
       <c r="N23" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O23" s="66"/>
       <c r="P23" s="55" t="s">
@@ -2584,7 +3388,7 @@
       </c>
       <c r="Q23" s="63"/>
       <c r="R23" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S23" s="35" t="s">
         <v>4</v>
@@ -2600,7 +3404,7 @@
       <c r="L24" s="58"/>
       <c r="M24" s="59"/>
       <c r="N24" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O24" s="67"/>
       <c r="P24" s="61"/>
@@ -2616,7 +3420,7 @@
       <c r="L25" s="58"/>
       <c r="M25" s="59"/>
       <c r="N25" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O25" s="67"/>
       <c r="P25" s="61"/>
@@ -2632,7 +3436,7 @@
       <c r="L26" s="50"/>
       <c r="M26" s="52"/>
       <c r="N26" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O26" s="68"/>
       <c r="P26" s="56"/>
@@ -2645,16 +3449,16 @@
     </row>
     <row r="27" spans="11:22" ht="54" x14ac:dyDescent="0.35">
       <c r="K27" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="L27" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="M27" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="L27" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="M27" s="51" t="s">
-        <v>56</v>
-      </c>
       <c r="N27" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O27" s="53"/>
       <c r="P27" s="55" t="s">
@@ -2671,7 +3475,7 @@
         <v>45303</v>
       </c>
       <c r="U27" s="90" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="V27" s="41"/>
     </row>
@@ -2680,7 +3484,7 @@
       <c r="L28" s="58"/>
       <c r="M28" s="59"/>
       <c r="N28" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O28" s="60"/>
       <c r="P28" s="61"/>
@@ -2696,7 +3500,7 @@
       <c r="L29" s="58"/>
       <c r="M29" s="59"/>
       <c r="N29" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O29" s="60"/>
       <c r="P29" s="61"/>
@@ -2737,16 +3541,16 @@
     </row>
     <row r="32" spans="11:22" ht="40.5" x14ac:dyDescent="0.35">
       <c r="K32" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="L32" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="L32" s="49" t="s">
+      <c r="M32" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="M32" s="51" t="s">
+      <c r="N32" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="N32" s="8" t="s">
-        <v>60</v>
       </c>
       <c r="O32" s="53"/>
       <c r="P32" s="55" t="s">
@@ -2770,7 +3574,7 @@
       <c r="L33" s="50"/>
       <c r="M33" s="52"/>
       <c r="N33" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O33" s="54"/>
       <c r="P33" s="56"/>
@@ -2783,22 +3587,22 @@
     </row>
     <row r="34" spans="11:22" ht="81.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K34" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="L34" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="M34" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="L34" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="M34" s="12" t="s">
-        <v>63</v>
-      </c>
       <c r="N34" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O34" s="15"/>
       <c r="P34" s="16"/>
       <c r="Q34" s="17"/>
       <c r="R34" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S34" s="7" t="s">
         <v>4</v>
@@ -2807,20 +3611,20 @@
         <v>45303</v>
       </c>
       <c r="U34" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="V34" s="18"/>
     </row>
     <row r="35" spans="11:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K35" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L35" s="14"/>
       <c r="M35" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N35" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O35" s="6"/>
       <c r="P35" s="16" t="s">
@@ -2828,7 +3632,7 @@
       </c>
       <c r="Q35" s="7"/>
       <c r="R35" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S35" s="7"/>
       <c r="T35" s="7"/>
@@ -2837,11 +3641,11 @@
     </row>
     <row r="36" spans="11:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K36" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L36" s="14"/>
       <c r="M36" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N36" s="10"/>
       <c r="O36" s="6"/>
@@ -2855,11 +3659,11 @@
     </row>
     <row r="37" spans="11:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K37" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L37" s="14"/>
       <c r="M37" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N37" s="19"/>
       <c r="O37" s="20"/>
@@ -2873,7 +3677,7 @@
     </row>
     <row r="41" spans="11:22" x14ac:dyDescent="0.35">
       <c r="K41" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L41" s="32"/>
       <c r="M41" s="32"/>
@@ -2889,7 +3693,6 @@
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="M15:M17"/>
     <mergeCell ref="T15:T17"/>
     <mergeCell ref="K41:V41"/>
     <mergeCell ref="O4:R8"/>
@@ -2905,7 +3708,6 @@
     <mergeCell ref="U13:U14"/>
     <mergeCell ref="V13:V14"/>
     <mergeCell ref="K15:K17"/>
-    <mergeCell ref="L15:L17"/>
     <mergeCell ref="U15:U17"/>
     <mergeCell ref="V15:V17"/>
     <mergeCell ref="K18:K20"/>
@@ -2921,6 +3723,7 @@
     <mergeCell ref="O15:O17"/>
     <mergeCell ref="P15:P17"/>
     <mergeCell ref="R15:R17"/>
+    <mergeCell ref="M15:M17"/>
     <mergeCell ref="S15:S17"/>
     <mergeCell ref="Q21:Q22"/>
     <mergeCell ref="K23:K26"/>
@@ -2933,6 +3736,7 @@
     <mergeCell ref="M21:M22"/>
     <mergeCell ref="O21:O22"/>
     <mergeCell ref="P21:P22"/>
+    <mergeCell ref="L15:L17"/>
     <mergeCell ref="U23:U26"/>
     <mergeCell ref="V23:V26"/>
     <mergeCell ref="R21:R22"/>
@@ -2982,7 +3786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BF5B63-E62D-4C4E-9431-2A5A77AD7493}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>